<commit_message>
added new label column to test data
</commit_message>
<xml_diff>
--- a/corehq/apps/data_dictionary/tests/data/clean_data_dictionary.xlsx
+++ b/corehq/apps/data_dictionary/tests/data/clean_data_dictionary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="caseType1" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="24">
   <si>
     <t xml:space="preserve">Case Property</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Label</t>
   </si>
   <si>
     <t xml:space="preserve">Deprecated</t>
@@ -167,12 +170,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -189,81 +196,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="10.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="n">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -272,7 +282,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -284,71 +294,71 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="29.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="18.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="31.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="29.31"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="C3" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>17</v>
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="0" t="n">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>18</v>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -357,75 +367,78 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="n">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -434,62 +447,62 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.2890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="36.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="32.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="32.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="37.8"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>